<commit_message>
push excel lkpbu 312 --> rata kanan
</commit_message>
<xml_diff>
--- a/assets/template-excel/template-lkpbu-312.xlsx
+++ b/assets/template-excel/template-lkpbu-312.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\reporting\assets\template-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D6CD4E7-1F76-4EE8-B536-05C853B1D648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F3CC28-2B74-4CD7-B47E-2002BBED0955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EB2135EB-6D1F-41F6-991F-9E778EF5CEEC}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{EB2135EB-6D1F-41F6-991F-9E778EF5CEEC}"/>
   </bookViews>
   <sheets>
     <sheet name="F312" sheetId="1" r:id="rId1"/>
@@ -608,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -646,56 +646,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -749,40 +728,55 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1101,7 +1095,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,10 +1104,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1229,18 +1223,18 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="16"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="22"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1257,17 +1251,17 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="18"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="51"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="51"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1288,26 +1282,26 @@
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="20" t="s">
+      <c r="D7" s="43"/>
+      <c r="E7" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23" t="s">
+      <c r="F7" s="53"/>
+      <c r="G7" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="20" t="s">
+      <c r="H7" s="43"/>
+      <c r="I7" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="20" t="s">
+      <c r="J7" s="43"/>
+      <c r="K7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="24"/>
+      <c r="L7" s="44"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1328,24 +1322,24 @@
       <c r="B8" s="7">
         <v>777930008</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="20" t="s">
+      <c r="D8" s="43"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="20">
+      <c r="H8" s="43"/>
+      <c r="I8" s="42">
         <v>312</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="20">
+      <c r="J8" s="43"/>
+      <c r="K8" s="42">
         <v>5</v>
       </c>
-      <c r="L8" s="24"/>
+      <c r="L8" s="44"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -1363,23 +1357,23 @@
     </row>
     <row r="9" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28" t="s">
+      <c r="C9" s="46"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="20" t="s">
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="24"/>
+      <c r="L9" s="44"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -1397,21 +1391,21 @@
     </row>
     <row r="10" spans="1:26" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="42" t="s">
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="43"/>
+      <c r="L10" s="36"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1429,21 +1423,21 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="47" t="s">
+      <c r="C11" s="38"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="48"/>
+      <c r="L11" s="41"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1461,21 +1455,21 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="49" t="s">
+      <c r="C12" s="38"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="50"/>
+      <c r="L12" s="41"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1493,21 +1487,21 @@
     </row>
     <row r="13" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="49" t="s">
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="50"/>
+      <c r="L13" s="41"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1525,21 +1519,21 @@
     </row>
     <row r="14" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="57" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="58"/>
+      <c r="L14" s="20"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1585,8 +1579,8 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -29177,6 +29171,30 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:J14"/>
     <mergeCell ref="K14:L14"/>
@@ -29190,30 +29208,6 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="K13:L13"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>